<commit_message>
Add D6 Hardware Naming
</commit_message>
<xml_diff>
--- a/Docs/API-SQL_Channel_Map.xlsx
+++ b/Docs/API-SQL_Channel_Map.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t xml:space="preserve">API</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t xml:space="preserve">Flowswitch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LevelSense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generic (D6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Levelsense</t>
   </si>
   <si>
     <t xml:space="preserve">R1</t>
@@ -172,6 +184,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -194,12 +207,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -256,19 +271,19 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -277,11 +292,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -289,11 +300,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -314,36 +325,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -363,10 +374,10 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -377,10 +388,10 @@
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -391,10 +402,10 @@
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -405,10 +416,10 @@
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -419,10 +430,10 @@
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -433,10 +444,10 @@
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -447,13 +458,13 @@
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -464,13 +475,13 @@
       <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
@@ -479,13 +490,13 @@
       <c r="B11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
@@ -494,92 +505,106 @@
       <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9" t="s">
+      <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+      <c r="D13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="7" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9"/>
+      <c r="B14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9"/>
+      <c r="A15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="9"/>
+      <c r="A16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9"/>
+      <c r="A17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
+      <c r="A18" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="9"/>
+      <c r="A19" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E9:E11"/>
-    <mergeCell ref="E13:E19"/>
+    <mergeCell ref="E14:E20"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>